<commit_message>
Fixed all DRC errors
</commit_message>
<xml_diff>
--- a/hardware_design/SEEDS/Project Outputs for SEEDS/SEEDS_BOM.xlsx
+++ b/hardware_design/SEEDS/Project Outputs for SEEDS/SEEDS_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="253">
   <si>
     <t>Description</t>
   </si>
@@ -771,6 +771,18 @@
   </si>
   <si>
     <t>18 </t>
+  </si>
+  <si>
+    <t>SLMD121H04L-ND</t>
+  </si>
+  <si>
+    <t>S7000-ND</t>
+  </si>
+  <si>
+    <t>S7036-ND</t>
+  </si>
+  <si>
+    <t>HM1168-ND</t>
   </si>
 </sst>
 </file>
@@ -1152,14 +1164,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="67.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
     <col min="7" max="9" width="11.109375" customWidth="1"/>
     <col min="10" max="10" width="20.44140625" customWidth="1"/>
     <col min="11" max="11" width="9.21875" customWidth="1"/>
@@ -2445,7 +2457,7 @@
         <v>16</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="K36" s="6" t="s">
         <v>180</v>
@@ -2479,7 +2491,7 @@
         <v>16</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="K37" t="s">
         <v>184</v>
@@ -2513,7 +2525,7 @@
         <v>16</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>173</v>
+        <v>251</v>
       </c>
       <c r="K38" t="s">
         <v>187</v>
@@ -2547,7 +2559,7 @@
         <v>16</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="K39" s="6" t="s">
         <v>191</v>

</xml_diff>